<commit_message>
update demo file format
</commit_message>
<xml_diff>
--- a/public/Student-Bulk-Import-Sample.xlsx
+++ b/public/Student-Bulk-Import-Sample.xlsx
@@ -27,7 +27,21 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Only unique number and maximum 9 digits.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +71,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Students ID</t>
+  </si>
   <si>
     <t xml:space="preserve">Student Name</t>
   </si>
@@ -208,39 +225,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="7.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -256,13 +273,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
       <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
@@ -273,8 +293,11 @@
       <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>8801770000000</v>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>8801700000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>